<commit_message>
update payroll and system
</commit_message>
<xml_diff>
--- a/src/assets/OPRFileImport/(OPR)Import Payroll/(OPR)Import Payroll Bonus.xlsx
+++ b/src/assets/OPRFileImport/(OPR)Import Payroll/(OPR)Import Payroll Bonus.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF48083-D092-4346-A253-6200F0B61E17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F5B978-5973-4CCE-B6E4-FEC41447D661}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>company_code</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>item_code</t>
-  </si>
-  <si>
-    <t>เลขที่  (null)</t>
   </si>
   <si>
     <t>ชื่อ ภาษาไทย ความยาวไม่เกิน 200 ตัว</t>
@@ -58,6 +55,15 @@
   </si>
   <si>
     <t>รหัสบริษัท</t>
+  </si>
+  <si>
+    <t>เป็นค่าว่างได้</t>
+  </si>
+  <si>
+    <t>เพิ่มข้อมูล ต้องไม่เป็นค่าว่าง</t>
+  </si>
+  <si>
+    <t>เลขที่  (null)  ตัวเลขเท่านั้น</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
@@ -163,6 +169,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -448,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,39 +502,42 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB3052E-8483-49FC-8994-A91D642A4015}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="20.81640625" customWidth="1"/>
     <col min="6" max="6" width="25.6328125" customWidth="1"/>
+    <col min="8" max="9" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -544,8 +556,17 @@
       <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>